<commit_message>
Status for CARBON-367, CARBON-368 & CARBON-154.
</commit_message>
<xml_diff>
--- a/Tickets_tested.xlsx
+++ b/Tickets_tested.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95">
   <si>
     <t>Sprint No</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>After fix raised ticket 3rd time</t>
+  </si>
+  <si>
+    <t>After fix raised ticket 4th time</t>
   </si>
   <si>
     <t>Sprint-77</t>
@@ -211,6 +214,9 @@
     <t>OS Carbon: Remove Main Partner from “Attach Partner Property” Dropdown</t>
   </si>
   <si>
+    <t>After fixing it after 4th time tested it on Harsh's VM.(do avoid rework)</t>
+  </si>
+  <si>
     <t>Harsh</t>
   </si>
   <si>
@@ -235,13 +241,34 @@
     <t>Defect_Report_CARBON-367_V2</t>
   </si>
   <si>
-    <t>Even after testing it twice found a defect.</t>
+    <t>Yes raised a ticket after fixing the defect 4th time.</t>
+  </si>
+  <si>
+    <t>Defect_Report_CARBON-367_V3</t>
+  </si>
+  <si>
+    <t>Even after testing it four times found a defect.</t>
   </si>
   <si>
     <t>CARBON-368</t>
   </si>
   <si>
     <t>OS Carbon: “Attach to Partner Property” Dropdown Permissions</t>
+  </si>
+  <si>
+    <t>After fixing it twice tested it on Harsh's VM.(do avoid rework)</t>
+  </si>
+  <si>
+    <t>Found a defect in working functionality of the page.</t>
+  </si>
+  <si>
+    <t>Yes, Twice.</t>
+  </si>
+  <si>
+    <t>Defect_Report_CARBON_368</t>
+  </si>
+  <si>
+    <t>Defect_Report_CARBON_368_V2</t>
   </si>
   <si>
     <t>CARBON-34</t>
@@ -273,6 +300,15 @@
   </si>
   <si>
     <t>Client Numbers: Existing client number should be edited/deleted without throwing any error</t>
+  </si>
+  <si>
+    <t>Was not able to reproduce as it was related to account which was deleted.</t>
+  </si>
+  <si>
+    <t>Yes. But its not related to the expected working of ticket. Related to another account on the same page.</t>
+  </si>
+  <si>
+    <t>While testing it with other scenarios could not find any client numbers under 74023, as they are already deleted. So not able to understand the actual working of the defect.</t>
   </si>
 </sst>
 </file>
@@ -280,10 +316,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -345,14 +381,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -497,6 +533,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -515,6 +557,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -533,6 +581,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -545,6 +599,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -575,25 +635,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,6 +683,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -635,49 +707,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,7 +844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -826,134 +862,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -999,6 +1035,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1016,6 +1055,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1331,10 +1376,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1344,14 +1389,14 @@
     <col min="4" max="5" width="11.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="12.1428571428571" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="9" max="9" width="13.7142857142857" customWidth="1"/>
     <col min="10" max="10" width="33.8571428571429" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="12.2857142857143" customWidth="1"/>
+    <col min="15" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="12.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="60" spans="1:15">
+    <row r="1" ht="60" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1379,50 +1424,65 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="O1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="S1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" ht="110.25" spans="1:15">
+    <row r="2" ht="110.25" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -1430,30 +1490,35 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
     </row>
-    <row r="3" ht="78.75" spans="1:15">
+    <row r="3" ht="78.75" spans="1:20">
       <c r="A3" s="7"/>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -1461,30 +1526,35 @@
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
     </row>
-    <row r="4" ht="78.75" spans="1:15">
+    <row r="4" ht="78.75" spans="1:20">
       <c r="A4" s="7"/>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -1492,32 +1562,37 @@
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
     </row>
-    <row r="5" ht="63" spans="1:15">
+    <row r="5" ht="63" spans="1:20">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -1525,30 +1600,35 @@
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
     </row>
-    <row r="6" ht="63" spans="1:15">
+    <row r="6" ht="63" spans="1:20">
       <c r="A6" s="7"/>
       <c r="B6" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -1556,30 +1636,35 @@
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
     </row>
-    <row r="7" ht="78.75" spans="1:15">
+    <row r="7" ht="78.75" spans="1:20">
       <c r="A7" s="7"/>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1587,30 +1672,35 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
     </row>
-    <row r="8" ht="105" spans="1:15">
+    <row r="8" ht="105" spans="1:20">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -1618,98 +1708,113 @@
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
     </row>
-    <row r="9" ht="60" spans="1:15">
+    <row r="9" ht="60" spans="1:20">
       <c r="A9" s="7"/>
       <c r="B9" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="20" t="s">
         <v>43</v>
       </c>
+      <c r="J9" s="21" t="s">
+        <v>44</v>
+      </c>
       <c r="K9" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
     </row>
-    <row r="10" ht="60" spans="1:15">
+    <row r="10" ht="60" spans="1:20">
       <c r="A10" s="7"/>
       <c r="B10" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
     </row>
-    <row r="11" ht="45" spans="1:15">
+    <row r="11" ht="45" spans="1:20">
       <c r="A11" s="7"/>
       <c r="B11" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
@@ -1717,30 +1822,35 @@
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
     </row>
-    <row r="12" ht="75" spans="1:15">
+    <row r="12" ht="75" spans="1:20">
       <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -1748,27 +1858,32 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
     </row>
-    <row r="13" ht="57" spans="1:15">
+    <row r="13" ht="57" spans="1:20">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -1777,122 +1892,166 @@
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
     </row>
-    <row r="14" ht="105" spans="1:15">
+    <row r="14" ht="105" spans="1:20">
       <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="E14" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>67</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M14" s="10" t="s">
         <v>68</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="R14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
     </row>
-    <row r="15" ht="71.25" spans="1:15">
+    <row r="15" ht="105" spans="1:20">
       <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>77</v>
+      </c>
       <c r="E15" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="7"/>
+        <v>60</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+      <c r="K15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
     </row>
-    <row r="16" ht="120" spans="1:15">
+    <row r="16" ht="90" spans="1:20">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="G16" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="10" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
     </row>
-    <row r="17" ht="90" spans="1:15">
+    <row r="17" ht="90" spans="1:20">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="G17" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -1901,23 +2060,28 @@
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
     </row>
-    <row r="18" ht="94.5" spans="1:15">
+    <row r="18" ht="94.5" spans="1:20">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>80</v>
+        <v>88</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -1926,34 +2090,50 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
     </row>
-    <row r="19" ht="108" customHeight="1" spans="1:15">
+    <row r="19" ht="162" customHeight="1" spans="1:20">
       <c r="A19" s="7"/>
-      <c r="B19" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="7"/>
+      <c r="B19" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="E19" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+        <v>60</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
     </row>
     <row r="23" ht="17.25" spans="5:5">
-      <c r="E23" s="18"/>
+      <c r="E23" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Added tickets for Sprint-80
</commit_message>
<xml_diff>
--- a/Tickets_tested.xlsx
+++ b/Tickets_tested.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15990" windowHeight="8100"/>
+    <workbookView windowWidth="20385" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104">
   <si>
     <t>Sprint No</t>
   </si>
@@ -214,7 +214,7 @@
     <t>OS Carbon: Remove Main Partner from “Attach Partner Property” Dropdown</t>
   </si>
   <si>
-    <t>After fixing it after 4th time tested it on Harsh's VM.(do avoid rework)</t>
+    <t>After fixing it after 4th time tested it on Harsh's VM.(to avoid rework)</t>
   </si>
   <si>
     <t>Harsh</t>
@@ -250,13 +250,16 @@
     <t>Even after testing it four times found a defect.</t>
   </si>
   <si>
+    <t>After fixing it for 4th time tested on Harsh VM machine before pushing to dev. (To avoid rework)</t>
+  </si>
+  <si>
     <t>CARBON-368</t>
   </si>
   <si>
     <t>OS Carbon: “Attach to Partner Property” Dropdown Permissions</t>
   </si>
   <si>
-    <t>After fixing it twice tested it on Harsh's VM.(do avoid rework)</t>
+    <t>After fixing it twice tested it on Harsh's VM.(to avoid rework)</t>
   </si>
   <si>
     <t>Found a defect in working functionality of the page.</t>
@@ -309,6 +312,30 @@
   </si>
   <si>
     <t>While testing it with other scenarios could not find any client numbers under 74023, as they are already deleted. So not able to understand the actual working of the defect.</t>
+  </si>
+  <si>
+    <t>Sprint-80</t>
+  </si>
+  <si>
+    <t>CARBON-369</t>
+  </si>
+  <si>
+    <t>OS Carbon: Price and Cost Changes</t>
+  </si>
+  <si>
+    <t>Om &amp; Abhay</t>
+  </si>
+  <si>
+    <t>CARBON-381</t>
+  </si>
+  <si>
+    <t>OS Valencia: Roadmap Admin Number</t>
+  </si>
+  <si>
+    <t>CARBON-382</t>
+  </si>
+  <si>
+    <t>OS Valencia: Case Admin Number</t>
   </si>
 </sst>
 </file>
@@ -316,12 +343,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +399,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <u/>
       <sz val="13.5"/>
@@ -381,14 +414,70 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -402,11 +491,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -417,32 +519,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -455,74 +556,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -533,6 +566,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -557,6 +596,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -581,6 +650,90 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -594,126 +747,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -742,36 +775,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -787,21 +794,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -812,6 +804,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -839,12 +846,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -862,134 +895,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1035,32 +1068,41 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1378,8 +1420,8 @@
   <sheetPr/>
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1394,6 +1436,7 @@
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="15" max="17" width="12" customWidth="1"/>
     <col min="18" max="18" width="12.2857142857143" customWidth="1"/>
+    <col min="19" max="19" width="11.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="60" spans="1:20">
@@ -1424,37 +1467,37 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="T1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1493,8 +1536,8 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
     </row>
     <row r="3" ht="78.75" spans="1:20">
       <c r="A3" s="7"/>
@@ -1529,8 +1572,8 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" ht="78.75" spans="1:20">
       <c r="A4" s="7"/>
@@ -1565,8 +1608,8 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
     </row>
     <row r="5" ht="63" spans="1:20">
       <c r="A5" s="1" t="s">
@@ -1603,8 +1646,8 @@
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
     </row>
     <row r="6" ht="63" spans="1:20">
       <c r="A6" s="7"/>
@@ -1639,8 +1682,8 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
     </row>
     <row r="7" ht="78.75" spans="1:20">
       <c r="A7" s="7"/>
@@ -1675,8 +1718,8 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
     </row>
     <row r="8" ht="105" spans="1:20">
       <c r="A8" s="7"/>
@@ -1711,8 +1754,8 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
     </row>
     <row r="9" ht="60" spans="1:20">
       <c r="A9" s="7"/>
@@ -1738,7 +1781,7 @@
       <c r="I9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="25" t="s">
         <v>44</v>
       </c>
       <c r="K9" s="10" t="s">
@@ -1751,8 +1794,8 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
     </row>
     <row r="10" ht="60" spans="1:20">
       <c r="A10" s="7"/>
@@ -1789,8 +1832,8 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
     </row>
     <row r="11" ht="45" spans="1:20">
       <c r="A11" s="7"/>
@@ -1825,8 +1868,8 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
     </row>
     <row r="12" ht="75" spans="1:20">
       <c r="A12" s="7"/>
@@ -1861,8 +1904,8 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
     </row>
     <row r="13" ht="57" spans="1:20">
       <c r="A13" s="1" t="s">
@@ -1895,10 +1938,10 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
     </row>
-    <row r="14" ht="105" spans="1:20">
+    <row r="14" ht="165" spans="1:20">
       <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>61</v>
@@ -1906,7 +1949,7 @@
       <c r="C14" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="8" t="s">
@@ -1922,7 +1965,7 @@
       <c r="I14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="25" t="s">
         <v>67</v>
       </c>
       <c r="K14" s="10" t="s">
@@ -1949,58 +1992,62 @@
       <c r="R14" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
+      <c r="S14" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="T14" s="7"/>
     </row>
-    <row r="15" ht="105" spans="1:20">
+    <row r="15" ht="165" spans="1:20">
       <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="15" t="s">
         <v>77</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>64</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="10" t="s">
         <v>60</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>69</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
+      <c r="S15" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="T15" s="7"/>
     </row>
     <row r="16" ht="90" spans="1:20">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
@@ -2016,11 +2063,11 @@
         <v>60</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
@@ -2029,16 +2076,16 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
     </row>
     <row r="17" ht="90" spans="1:20">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
@@ -2063,16 +2110,16 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
     </row>
     <row r="18" ht="94.5" spans="1:20">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="16" t="s">
         <v>89</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
@@ -2093,19 +2140,19 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
     </row>
     <row r="19" ht="162" customHeight="1" spans="1:20">
       <c r="A19" s="7"/>
-      <c r="B19" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>91</v>
       </c>
+      <c r="C19" s="17" t="s">
+        <v>92</v>
+      </c>
       <c r="D19" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>17</v>
@@ -2116,10 +2163,10 @@
         <v>60</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
@@ -2129,11 +2176,97 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" ht="40" customHeight="1" spans="1:20">
+      <c r="A20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+    </row>
+    <row r="21" ht="49" customHeight="1" spans="1:20">
+      <c r="A21" s="20"/>
+      <c r="B21" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="20"/>
+    </row>
+    <row r="22" ht="31.5" spans="1:20">
+      <c r="A22" s="20"/>
+      <c r="B22" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
     </row>
     <row r="23" ht="17.25" spans="5:5">
-      <c r="E23" s="19"/>
+      <c r="E23" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Added report for tickets tested on QA.
</commit_message>
<xml_diff>
--- a/Tickets_tested.xlsx
+++ b/Tickets_tested.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105">
   <si>
     <t>Sprint No</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Found a defect in the working functionality of the page.</t>
+  </si>
+  <si>
+    <t>Tested on QA, but the ticket is not working properly.</t>
   </si>
   <si>
     <t>Yes, discussed with client also. Found one more defect.</t>
@@ -344,9 +347,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -414,7 +417,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -428,6 +446,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -452,6 +477,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -469,6 +509,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -477,22 +525,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -513,29 +546,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -548,14 +559,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -566,36 +569,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -608,61 +677,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -686,67 +749,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,6 +778,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -786,9 +804,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -808,17 +852,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -837,47 +875,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -895,134 +898,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1068,6 +1071,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1077,18 +1083,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1100,9 +1097,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1420,8 +1414,8 @@
   <sheetPr/>
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1467,34 +1461,34 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="Q1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="24" t="s">
+      <c r="S1" s="22" t="s">
         <v>13</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -1781,7 +1775,7 @@
       <c r="I9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="23" t="s">
         <v>44</v>
       </c>
       <c r="K9" s="10" t="s">
@@ -1958,96 +1952,100 @@
       <c r="F14" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="15" t="s">
+        <v>66</v>
+      </c>
       <c r="H14" s="10" t="s">
         <v>60</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" s="25" t="s">
         <v>67</v>
       </c>
+      <c r="J14" s="23" t="s">
+        <v>68</v>
+      </c>
       <c r="K14" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L14" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="M14" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="N14" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="S14" s="26" t="s">
         <v>75</v>
+      </c>
+      <c r="S14" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="T14" s="7"/>
     </row>
     <row r="15" ht="165" spans="1:20">
       <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>64</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="7"/>
+        <v>80</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>66</v>
+      </c>
       <c r="H15" s="10" t="s">
         <v>60</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
-      <c r="S15" s="26" t="s">
-        <v>75</v>
+      <c r="S15" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="T15" s="7"/>
     </row>
     <row r="16" ht="90" spans="1:20">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
@@ -2056,18 +2054,18 @@
       <c r="F16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>18</v>
+      <c r="G16" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>60</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
@@ -2082,10 +2080,10 @@
     <row r="17" ht="90" spans="1:20">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
@@ -2094,8 +2092,8 @@
       <c r="F17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>49</v>
+      <c r="G17" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>60</v>
@@ -2116,10 +2114,10 @@
     <row r="18" ht="94.5" spans="1:20">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="15" t="s">
         <v>90</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
@@ -2145,14 +2143,14 @@
     </row>
     <row r="19" ht="162" customHeight="1" spans="1:20">
       <c r="A19" s="7"/>
-      <c r="B19" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="17" t="s">
         <v>92</v>
       </c>
+      <c r="C19" s="18" t="s">
+        <v>93</v>
+      </c>
       <c r="D19" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>17</v>
@@ -2163,10 +2161,10 @@
         <v>60</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
@@ -2181,92 +2179,92 @@
     </row>
     <row r="20" ht="40" customHeight="1" spans="1:20">
       <c r="A20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="18" t="s">
         <v>97</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="C20" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
     </row>
     <row r="21" ht="49" customHeight="1" spans="1:20">
-      <c r="A21" s="20"/>
-      <c r="B21" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="22" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21" t="s">
+      <c r="C21" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="20"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
     </row>
     <row r="22" ht="31.5" spans="1:20">
-      <c r="A22" s="20"/>
-      <c r="B22" s="18" t="s">
-        <v>102</v>
+      <c r="A22" s="7"/>
+      <c r="B22" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
     </row>
     <row r="23" ht="17.25" spans="5:5">
-      <c r="E23" s="23"/>
+      <c r="E23" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Updated for tickets AgileZen#381 & AgileZen#382
</commit_message>
<xml_diff>
--- a/Tickets_tested.xlsx
+++ b/Tickets_tested.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124">
   <si>
     <t>Sprint No</t>
   </si>
@@ -368,22 +368,34 @@
     <t>Sprint-80</t>
   </si>
   <si>
-    <t>CARBON-369</t>
+    <t>AgileZen # 381</t>
+  </si>
+  <si>
+    <t>OS Valencia: Roadmap Admin Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Found a defect </t>
+  </si>
+  <si>
+    <t>AgileZen # 382</t>
+  </si>
+  <si>
+    <t>OS Valencia: Case Admin Number</t>
+  </si>
+  <si>
+    <t>Found two defects.</t>
+  </si>
+  <si>
+    <t>Sprint-81</t>
+  </si>
+  <si>
+    <t>AgileZen # 369</t>
   </si>
   <si>
     <t>OS Carbon: Price and Cost Changes</t>
   </si>
   <si>
-    <t>CARBON-381</t>
-  </si>
-  <si>
-    <t>OS Valencia: Roadmap Admin Number</t>
-  </si>
-  <si>
-    <t>CARBON-382</t>
-  </si>
-  <si>
-    <t>OS Valencia: Case Admin Number</t>
+    <t>Om &amp; Harsh</t>
   </si>
 </sst>
 </file>
@@ -396,7 +408,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,70 +465,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="13.5"/>
-      <color rgb="FF0000FF"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -531,9 +481,32 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -555,7 +528,38 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -566,6 +570,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -584,20 +596,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -614,6 +618,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -626,25 +684,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,54 +708,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -722,6 +726,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -734,12 +768,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -752,36 +780,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -789,12 +799,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,6 +827,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -840,44 +877,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -925,152 +929,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1129,25 +1133,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1463,15 +1461,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O19" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="18.5714285714286" customWidth="1"/>
     <col min="4" max="5" width="11.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
@@ -1611,10 +1609,10 @@
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
     </row>
     <row r="3" ht="78.75" spans="1:28">
       <c r="A3" s="8"/>
@@ -1655,10 +1653,10 @@
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
     </row>
     <row r="4" ht="78.75" spans="1:28">
       <c r="A4" s="8"/>
@@ -1699,10 +1697,10 @@
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
     </row>
     <row r="5" ht="63" spans="1:28">
       <c r="A5" s="1" t="s">
@@ -1745,10 +1743,10 @@
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="24"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
     </row>
     <row r="6" ht="63" spans="1:28">
       <c r="A6" s="8"/>
@@ -1789,10 +1787,10 @@
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
     </row>
     <row r="7" ht="78.75" spans="1:28">
       <c r="A7" s="8"/>
@@ -1833,10 +1831,10 @@
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="24"/>
-      <c r="AB7" s="24"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
     </row>
     <row r="8" ht="105" spans="1:28">
       <c r="A8" s="8"/>
@@ -1877,10 +1875,10 @@
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
     </row>
     <row r="9" ht="60" spans="1:28">
       <c r="A9" s="8"/>
@@ -1925,10 +1923,10 @@
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="24"/>
-      <c r="AB9" s="24"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
     </row>
     <row r="10" ht="60" spans="1:28">
       <c r="A10" s="8"/>
@@ -1971,10 +1969,10 @@
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="24"/>
-      <c r="AB10" s="24"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
     </row>
     <row r="11" ht="45" spans="1:28">
       <c r="A11" s="8"/>
@@ -2015,10 +2013,10 @@
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
       <c r="X11" s="8"/>
-      <c r="Y11" s="24"/>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="24"/>
-      <c r="AB11" s="24"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
     </row>
     <row r="12" ht="75" spans="1:28">
       <c r="A12" s="8"/>
@@ -2059,10 +2057,10 @@
       <c r="V12" s="8"/>
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="24"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
     </row>
     <row r="13" ht="57" spans="1:28">
       <c r="A13" s="1" t="s">
@@ -2102,10 +2100,10 @@
       <c r="V13" s="8"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8"/>
-      <c r="Y13" s="24"/>
-      <c r="Z13" s="24"/>
-      <c r="AA13" s="24"/>
-      <c r="AB13" s="24"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
     </row>
     <row r="14" ht="165" spans="1:28">
       <c r="A14" s="8"/>
@@ -2176,16 +2174,16 @@
         <v>87</v>
       </c>
       <c r="X14" s="8"/>
-      <c r="Y14" s="25" t="s">
+      <c r="Y14" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="Z14" s="25" t="s">
+      <c r="Z14" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="AA14" s="25" t="s">
+      <c r="AA14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="AB14" s="25" t="s">
+      <c r="AB14" s="11" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2240,10 +2238,10 @@
         <v>87</v>
       </c>
       <c r="X15" s="8"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
     </row>
     <row r="16" ht="105" spans="1:28">
       <c r="A16" s="8"/>
@@ -2288,10 +2286,10 @@
       <c r="V16" s="8"/>
       <c r="W16" s="8"/>
       <c r="X16" s="8"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
-      <c r="AA16" s="24"/>
-      <c r="AB16" s="24"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
     </row>
     <row r="17" ht="105" spans="1:28">
       <c r="A17" s="8"/>
@@ -2332,10 +2330,10 @@
       <c r="V17" s="8"/>
       <c r="W17" s="8"/>
       <c r="X17" s="8"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
     </row>
     <row r="18" ht="94.5" spans="1:28">
       <c r="A18" s="8"/>
@@ -2371,10 +2369,10 @@
       <c r="V18" s="8"/>
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="8"/>
     </row>
     <row r="19" ht="162" customHeight="1" spans="1:28">
       <c r="A19" s="8"/>
@@ -2415,34 +2413,26 @@
       <c r="V19" s="8"/>
       <c r="W19" s="8"/>
       <c r="X19" s="8"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
     </row>
-    <row r="20" ht="40" customHeight="1" spans="1:28">
-      <c r="A20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9" t="s">
-        <v>56</v>
-      </c>
+    <row r="20" ht="21" customHeight="1" spans="1:28">
+      <c r="A20" s="8"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
@@ -2453,24 +2443,28 @@
       <c r="V20" s="8"/>
       <c r="W20" s="8"/>
       <c r="X20" s="8"/>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
     </row>
     <row r="21" ht="49" customHeight="1" spans="1:28">
-      <c r="A21" s="8"/>
+      <c r="A21" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="B21" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="20" t="s">
+        <v>116</v>
+      </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
@@ -2489,24 +2483,26 @@
       <c r="V21" s="8"/>
       <c r="W21" s="8"/>
       <c r="X21" s="8"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="24"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
     </row>
     <row r="22" ht="31.5" spans="1:28">
       <c r="A22" s="8"/>
       <c r="B22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>118</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>119</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="20" t="s">
+        <v>119</v>
+      </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -2525,13 +2521,168 @@
       <c r="V22" s="8"/>
       <c r="W22" s="8"/>
       <c r="X22" s="8"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="24"/>
-      <c r="AB22" s="24"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
     </row>
-    <row r="23" ht="17.25" spans="5:5">
-      <c r="E23" s="21"/>
+    <row r="23" ht="15.75" spans="1:28">
+      <c r="A23" s="8"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+    </row>
+    <row r="24" ht="31.5" spans="1:28">
+      <c r="A24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8"/>
+    </row>
+    <row r="25" spans="1:28">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+      <c r="AB25" s="8"/>
+    </row>
+    <row r="26" spans="1:28">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="8"/>
+    </row>
+    <row r="27" spans="1:28">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="8"/>
+      <c r="AB27" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>